<commit_message>
Added distribution and plots folder
Added plots of variable distributions, more geographic plots, and reorganized datasets and plots locations
</commit_message>
<xml_diff>
--- a/data/EJI_DATADICTIONARY_2022.xlsx
+++ b/data/EJI_DATADICTIONARY_2022.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/xqe6_cdc_gov/Documents/Project_Data/EJI/Web_Files/Web_Files/Data_Dictionary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/debf4120bbe035ba/George Washington University/Spring 2025/STAT 6289 Spatial Statistics/spatial_statistics_final_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{479155AC-31C6-4280-B9E5-3177A359A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C00BCAD-08EC-4C37-8D7E-5350A424E5D5}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{479155AC-31C6-4280-B9E5-3177A359A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCD5491E-9946-4E2E-A884-7D5F6A5F42E5}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-6615" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3C4EE6-DF52-44F5-B414-D5B723B1F35A}"/>
+    <workbookView xWindow="12720" yWindow="0" windowWidth="12970" windowHeight="13770" xr2:uid="{6C3C4EE6-DF52-44F5-B414-D5B723B1F35A}"/>
   </bookViews>
   <sheets>
     <sheet name="EJI_DATADICTIONARY_2022" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EJI_DATADICTIONARY_2022!$A$1:$A$119</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1248,72 +1251,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1345,9 +1342,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1385,7 +1382,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1491,7 +1488,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1633,7 +1630,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1641,55 +1638,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E54FD2A-08AE-4F53-B9A2-B079206BD1D4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="63" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="63" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="106.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="70.1796875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="106.453125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="27.54296875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="1" customWidth="1"/>
     <col min="9" max="9" width="26" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="1" customWidth="1"/>
-    <col min="14" max="15" width="8.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="1" customWidth="1"/>
-    <col min="19" max="22" width="7.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="7.28515625" style="1" customWidth="1"/>
-    <col min="24" max="27" width="9.28515625" style="1" customWidth="1"/>
-    <col min="28" max="29" width="10.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="9.42578125" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="20.7109375" style="1"/>
+    <col min="10" max="10" width="8.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="8.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.54296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1796875" style="1" customWidth="1"/>
+    <col min="19" max="22" width="7.453125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="7.26953125" style="1" customWidth="1"/>
+    <col min="24" max="27" width="9.26953125" style="1" customWidth="1"/>
+    <col min="28" max="29" width="10.54296875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="9.453125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="20.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1698,21 +1696,21 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1721,21 +1719,21 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1744,21 +1742,21 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1767,21 +1765,21 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1790,21 +1788,21 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1813,21 +1811,21 @@
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1836,21 +1834,21 @@
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1859,21 +1857,21 @@
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1882,21 +1880,21 @@
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1905,21 +1903,21 @@
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1928,21 +1926,21 @@
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1951,21 +1949,21 @@
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1974,21 +1972,21 @@
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1997,21 +1995,21 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="E15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2020,21 +2018,21 @@
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="13" t="s">
+      <c r="E16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2043,21 +2041,21 @@
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="E17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2066,2340 +2064,2391 @@
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="13" t="s">
+      <c r="E18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="G18" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="F19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="G20" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G22" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="G22" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="F23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="15" t="s">
+      <c r="E24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G24" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="G24" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="F25" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="15" t="s">
+      <c r="E26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="G26" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="G26" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="F27" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="15" t="s">
+      <c r="E28" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="G28" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="F29" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G30" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="G30" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="F31" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="15" t="s">
+      <c r="E32" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="G32" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="G32" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="F33" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="E34" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="G34" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="F35" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="15" t="s">
+      <c r="E36" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="G36" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="G36" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="15" t="s">
+      <c r="E37" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
+      <c r="E38" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="G38" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="G38" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E40" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="14" t="s">
+      <c r="E40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="G40" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="G40" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="F41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="14" t="s">
+      <c r="E42" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="G42" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="G42" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="F43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="14" t="s">
+      <c r="E44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G44" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="G44" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="F45" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="14" t="s">
+      <c r="E46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="G46" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="G46" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E47" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="14" t="s">
+      <c r="E47" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="14" t="s">
+      <c r="E48" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="G48" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="G48" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="F49" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="F49" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="15" t="s">
+      <c r="E50" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="G50" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="G50" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="F51" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="15" t="s">
+      <c r="E52" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="G52" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="G52" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="15" t="s">
+      <c r="E53" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+    <row r="54" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="15" t="s">
+      <c r="E54" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="G54" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="G54" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B55" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="7" t="s">
+      <c r="B55" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="14" t="s">
+      <c r="D55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+    <row r="56" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="14" t="s">
+      <c r="D56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="G56" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="G56" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="F57" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="F57" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="C58" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="16" t="s">
+      <c r="E58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G58" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="G58" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="5" t="s">
+      <c r="C59" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="F59" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="F59" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="5" t="s">
+      <c r="C60" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="16" t="s">
+      <c r="E60" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G60" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="G60" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="C61" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="F61" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="C62" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E62" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="16" t="s">
+      <c r="E62" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G62" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="G62" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="C63" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="F63" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="F63" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C64" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E64" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="16" t="s">
+      <c r="E64" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G64" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="G64" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E65" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="16" t="s">
+      <c r="E65" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G65" s="16" t="s">
+      <c r="G65" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E66" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="16" t="s">
+      <c r="E66" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="G66" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="C67" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="6" t="s">
+      <c r="C67" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="E67" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="F67" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="F67" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68" s="6" t="s">
+      <c r="C68" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E68" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="17" t="s">
+      <c r="E68" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G68" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="G68" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="C69" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E69" s="18" t="s">
+      <c r="E69" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="F69" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="F69" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="C70" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E70" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="17" t="s">
+      <c r="E70" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G70" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="G70" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="6" t="s">
+      <c r="C71" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E71" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="F71" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="F71" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72" s="6" t="s">
+      <c r="C72" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="17" t="s">
+      <c r="E72" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G72" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+      <c r="G72" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73" s="6" t="s">
+      <c r="C73" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E73" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="F73" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G73" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+      <c r="F73" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D74" s="6" t="s">
+      <c r="C74" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E74" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="17" t="s">
+      <c r="E74" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G74" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="G74" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="C75" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="F75" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G75" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="F75" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="C76" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="17" t="s">
+      <c r="E76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="G76" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" s="6" t="s">
+      <c r="C77" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E77" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="F77" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
+      <c r="F77" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" s="6" t="s">
+      <c r="C78" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="17" t="s">
+      <c r="E78" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G78" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+      <c r="G78" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="6" t="s">
+      <c r="C79" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E79" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="17" t="s">
+      <c r="E79" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="G79" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+    <row r="80" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D80" s="6" t="s">
+      <c r="C80" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E80" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="17" t="s">
+      <c r="E80" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G80" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="G80" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D81" s="5" t="s">
+      <c r="C81" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="E81" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="F81" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G81" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+      <c r="F81" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D82" s="5" t="s">
+      <c r="C82" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D82" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E82" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="16" t="s">
+      <c r="E82" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G82" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+      <c r="G82" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D83" s="5" t="s">
+      <c r="C83" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E83" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+      <c r="E83" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D84" s="5" t="s">
+      <c r="C84" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E84" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="16" t="s">
+      <c r="E84" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+      <c r="G84" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="5" t="s">
+      <c r="C85" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="F85" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="F85" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D86" s="5" t="s">
+      <c r="C86" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E86" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="16" t="s">
+      <c r="E86" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G86" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+      <c r="G86" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E87" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="16" t="s">
+      <c r="E87" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G87" s="16" t="s">
+      <c r="G87" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="88" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D88" s="5" t="s">
+      <c r="C88" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E88" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" s="16" t="s">
+      <c r="E88" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G88" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+      <c r="G88" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C89" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D89" s="6" t="s">
+      <c r="C89" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E89" s="17" t="s">
+      <c r="E89" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F89" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G89" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+      <c r="F89" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D90" s="6" t="s">
+      <c r="C90" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E90" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="17" t="s">
+      <c r="E90" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G90" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+      <c r="G90" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D91" s="6" t="s">
+      <c r="C91" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="17" t="s">
+      <c r="E91" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F91" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G91" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="F91" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D92" s="6" t="s">
+      <c r="C92" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E92" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="17" t="s">
+      <c r="E92" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="G92" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+      <c r="G92" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D93" s="6" t="s">
+      <c r="C93" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E93" s="17" t="s">
+      <c r="E93" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
+      <c r="F93" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D94" s="6" t="s">
+      <c r="C94" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E94" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" s="17" t="s">
+      <c r="E94" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="G94" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+      <c r="G94" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D95" s="6" t="s">
+      <c r="C95" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E95" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" s="17" t="s">
+      <c r="E95" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G95" s="17" t="s">
+      <c r="G95" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
+    <row r="96" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D96" s="6" t="s">
+      <c r="C96" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E96" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" s="17" t="s">
+      <c r="E96" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G96" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
+      <c r="G96" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="C97" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D97" s="5" t="s">
+      <c r="C97" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="F97" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G97" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+      <c r="F97" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="C98" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E98" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F98" s="16" t="s">
+      <c r="E98" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="G98" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+      <c r="G98" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="C99" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E99" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F99" s="16" t="s">
+      <c r="E99" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G99" s="16" t="s">
+      <c r="G99" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="100" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B100" s="16" t="s">
+      <c r="B100" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D100" s="5" t="s">
+      <c r="C100" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E100" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="16" t="s">
+      <c r="E100" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="G100" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="G100" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B101" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F101" s="17" t="s">
+      <c r="B101" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="G101" s="17" t="s">
+      <c r="G101" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+    <row r="102" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F102" s="17" t="s">
+      <c r="C102" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="G102" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
+      <c r="G102" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="B103" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D103" s="9" t="s">
+      <c r="D103" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E103" s="19" t="s">
+      <c r="E103" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F103" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
+      <c r="F103" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C104" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D104" s="10" t="s">
+      <c r="D104" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E104" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="20" t="s">
+      <c r="E104" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="G104" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
+      <c r="G104" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D105" s="9" t="s">
+      <c r="D105" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E105" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F105" s="19" t="s">
+      <c r="E105" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="G105" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="9" t="s">
+      <c r="G105" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B106" s="19" t="s">
+      <c r="B106" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D106" s="9" t="s">
+      <c r="D106" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E106" s="19" t="s">
+      <c r="E106" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F106" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G106" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
+      <c r="F106" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B107" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D107" s="9" t="s">
+      <c r="D107" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E107" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F107" s="19" t="s">
+      <c r="E107" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="G107" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
+      <c r="G107" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B108" s="19" t="s">
+      <c r="B108" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D108" s="9" t="s">
+      <c r="D108" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E108" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="19" t="s">
+      <c r="E108" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="G108" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
+      <c r="G108" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="B109" s="19" t="s">
+      <c r="B109" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D109" s="9" t="s">
+      <c r="D109" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E109" s="19" t="s">
+      <c r="E109" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F109" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G109" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+      <c r="F109" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B110" s="19" t="s">
+      <c r="B110" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D110" s="9" t="s">
+      <c r="D110" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E110" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F110" s="19" t="s">
+      <c r="E110" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="G110" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+      <c r="G110" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B111" s="19" t="s">
+      <c r="B111" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D111" s="9" t="s">
+      <c r="D111" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E111" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F111" s="19" t="s">
+      <c r="E111" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="G111" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+      <c r="G111" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="B112" s="19" t="s">
+      <c r="B112" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C112" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D112" s="9" t="s">
+      <c r="D112" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E112" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F112" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G112" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="9" t="s">
+      <c r="F112" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D113" s="9" t="s">
+      <c r="D113" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E113" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F113" s="19" t="s">
+      <c r="E113" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="G113" s="19" t="s">
+      <c r="G113" s="17" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
+    <row r="114" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B114" s="19" t="s">
+      <c r="B114" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D114" s="9" t="s">
+      <c r="D114" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E114" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F114" s="19" t="s">
+      <c r="E114" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="G114" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="9" t="s">
+      <c r="G114" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="B115" s="19" t="s">
+      <c r="B115" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="C115" s="9" t="s">
+      <c r="C115" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D115" s="9" t="s">
+      <c r="D115" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E115" s="19" t="s">
+      <c r="E115" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="F115" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G115" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="9" t="s">
+      <c r="F115" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B116" s="19" t="s">
+      <c r="B116" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D116" s="9" t="s">
+      <c r="D116" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E116" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F116" s="19" t="s">
+      <c r="E116" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="G116" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="9" t="s">
+      <c r="G116" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="C117" s="9" t="s">
+      <c r="C117" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D117" s="9" t="s">
+      <c r="D117" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E117" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F117" s="19" t="s">
+      <c r="E117" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="G117" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
+      <c r="G117" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="21" t="s">
+      <c r="B118" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E118" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F118" s="21" t="s">
+      <c r="D118" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="G118" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="11" t="s">
+      <c r="G118" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C119" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="D119" s="11" t="s">
+      <c r="D119" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="E119" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="21" t="s">
+      <c r="E119" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="G119" s="21" t="s">
+      <c r="G119" s="18" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A119" xr:uid="{8E54FD2A-08AE-4F53-B9A2-B079206BD1D4}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="2022 VARIABLE NAME"/>
+        <filter val="AFFGEOID"/>
+        <filter val="E_AIRPRT"/>
+        <filter val="E_COAL"/>
+        <filter val="E_DAYPOP"/>
+        <filter val="E_DSLPM"/>
+        <filter val="E_HOUAGE"/>
+        <filter val="E_IMPWTR"/>
+        <filter val="E_LEAD"/>
+        <filter val="E_NPL"/>
+        <filter val="E_OZONE"/>
+        <filter val="E_PARK"/>
+        <filter val="E_PM"/>
+        <filter val="E_RAIL"/>
+        <filter val="E_RMP"/>
+        <filter val="E_ROAD"/>
+        <filter val="E_TOTCR"/>
+        <filter val="E_TOTPOP"/>
+        <filter val="E_TRI"/>
+        <filter val="E_TSD"/>
+        <filter val="E_WLKIND"/>
+        <filter val="EP_AGE17"/>
+        <filter val="EP_AGE65"/>
+        <filter val="EP_ASTHMA"/>
+        <filter val="EP_BPHIGH"/>
+        <filter val="EP_CANCER"/>
+        <filter val="EP_DIABETES"/>
+        <filter val="EP_DISABL"/>
+        <filter val="EP_GROUPQ"/>
+        <filter val="EP_HOUBDN"/>
+        <filter val="EP_LIMENG"/>
+        <filter val="EP_MHLTH"/>
+        <filter val="EP_MINRTY"/>
+        <filter val="EP_MOBILE"/>
+        <filter val="EP_NOHSDP"/>
+        <filter val="EP_NOINT"/>
+        <filter val="EP_POV200"/>
+        <filter val="EP_RENTER"/>
+        <filter val="EP_UNEMP"/>
+        <filter val="EP_UNINSUR"/>
+        <filter val="GEOID"/>
+        <filter val="StateAbbr"/>
+        <filter val="StateDesc"/>
+        <filter val="STATEFP"/>
+        <filter val="TRACTCE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:G118">
     <sortCondition ref="C58:C118"/>
     <sortCondition ref="D58:D118"/>

</xml_diff>